<commit_message>
Third set of updates for HU
-including labour supply utility functions
</commit_message>
<xml_diff>
--- a/input/projections_fertility.xlsx
+++ b/input/projections_fertility.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\labsim\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E268E892-D14D-4480-8A90-D0AA4EA574E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1B676A-7A5C-4811-BDA7-30916E141B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1320" windowWidth="31350" windowHeight="16950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="UK_FertilityByYear" sheetId="3" r:id="rId2"/>
     <sheet name="IT_FertilityByYear" sheetId="4" r:id="rId3"/>
+    <sheet name="HU_FertilityByYear" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="88">
   <si>
     <t/>
   </si>
@@ -402,9 +403,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -442,7 +443,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -548,7 +549,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -690,7 +691,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -700,7 +701,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2061,7 +2062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC6C525-5E56-43D0-8485-7B36B4DC93F6}">
   <dimension ref="A1:BT2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BT1" sqref="B1:BT1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -2953,4 +2956,237 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F67E40-71C1-4822-9F58-EAF4B2A32D1B}">
+  <dimension ref="A1:AJ2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1">
+        <v>2011</v>
+      </c>
+      <c r="C1">
+        <v>2012</v>
+      </c>
+      <c r="D1">
+        <v>2013</v>
+      </c>
+      <c r="E1">
+        <v>2014</v>
+      </c>
+      <c r="F1">
+        <v>2015</v>
+      </c>
+      <c r="G1">
+        <v>2016</v>
+      </c>
+      <c r="H1">
+        <v>2017</v>
+      </c>
+      <c r="I1">
+        <v>2018</v>
+      </c>
+      <c r="J1">
+        <v>2019</v>
+      </c>
+      <c r="K1">
+        <v>2020</v>
+      </c>
+      <c r="L1">
+        <v>2021</v>
+      </c>
+      <c r="M1">
+        <v>2022</v>
+      </c>
+      <c r="N1">
+        <v>2023</v>
+      </c>
+      <c r="O1">
+        <v>2024</v>
+      </c>
+      <c r="P1">
+        <v>2025</v>
+      </c>
+      <c r="Q1">
+        <v>2026</v>
+      </c>
+      <c r="R1">
+        <v>2027</v>
+      </c>
+      <c r="S1">
+        <v>2028</v>
+      </c>
+      <c r="T1">
+        <v>2029</v>
+      </c>
+      <c r="U1">
+        <v>2030</v>
+      </c>
+      <c r="V1">
+        <v>2031</v>
+      </c>
+      <c r="W1">
+        <v>2032</v>
+      </c>
+      <c r="X1">
+        <v>2033</v>
+      </c>
+      <c r="Y1">
+        <v>2034</v>
+      </c>
+      <c r="Z1">
+        <v>2035</v>
+      </c>
+      <c r="AA1">
+        <v>2036</v>
+      </c>
+      <c r="AB1">
+        <v>2037</v>
+      </c>
+      <c r="AC1">
+        <v>2038</v>
+      </c>
+      <c r="AD1">
+        <v>2039</v>
+      </c>
+      <c r="AE1">
+        <v>2040</v>
+      </c>
+      <c r="AF1">
+        <v>2041</v>
+      </c>
+      <c r="AG1">
+        <v>2042</v>
+      </c>
+      <c r="AH1">
+        <v>2043</v>
+      </c>
+      <c r="AI1">
+        <v>2044</v>
+      </c>
+      <c r="AJ1">
+        <v>2045</v>
+      </c>
+    </row>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2">
+        <v>41</v>
+      </c>
+      <c r="C2">
+        <v>44.666666666666664</v>
+      </c>
+      <c r="D2">
+        <v>45.000000000000007</v>
+      </c>
+      <c r="E2">
+        <v>48</v>
+      </c>
+      <c r="F2">
+        <v>48.333333333333336</v>
+      </c>
+      <c r="G2">
+        <v>51.000000000000007</v>
+      </c>
+      <c r="H2">
+        <v>51.333333333333336</v>
+      </c>
+      <c r="I2">
+        <v>51.666666666666664</v>
+      </c>
+      <c r="J2">
+        <v>51.666666666666664</v>
+      </c>
+      <c r="K2">
+        <v>53.000000000000007</v>
+      </c>
+      <c r="L2">
+        <v>53.666666666666671</v>
+      </c>
+      <c r="M2">
+        <v>52.000000000000007</v>
+      </c>
+      <c r="N2">
+        <v>52.000000000000007</v>
+      </c>
+      <c r="O2">
+        <v>52.000000000000007</v>
+      </c>
+      <c r="P2">
+        <v>54.740666666666669</v>
+      </c>
+      <c r="Q2">
+        <v>54.740666666666669</v>
+      </c>
+      <c r="R2">
+        <v>54.740666666666669</v>
+      </c>
+      <c r="S2">
+        <v>54.740666666666669</v>
+      </c>
+      <c r="T2">
+        <v>54.740666666666669</v>
+      </c>
+      <c r="U2">
+        <v>55.614000000000004</v>
+      </c>
+      <c r="V2">
+        <v>55.614000000000004</v>
+      </c>
+      <c r="W2">
+        <v>55.614000000000004</v>
+      </c>
+      <c r="X2">
+        <v>55.614000000000004</v>
+      </c>
+      <c r="Y2">
+        <v>55.614000000000004</v>
+      </c>
+      <c r="Z2">
+        <v>56.212000000000003</v>
+      </c>
+      <c r="AA2">
+        <v>56.212000000000003</v>
+      </c>
+      <c r="AB2">
+        <v>56.212000000000003</v>
+      </c>
+      <c r="AC2">
+        <v>56.212000000000003</v>
+      </c>
+      <c r="AD2">
+        <v>56.212000000000003</v>
+      </c>
+      <c r="AE2">
+        <v>56.612000000000002</v>
+      </c>
+      <c r="AF2">
+        <v>56.612000000000002</v>
+      </c>
+      <c r="AG2">
+        <v>56.612000000000002</v>
+      </c>
+      <c r="AH2">
+        <v>56.612000000000002</v>
+      </c>
+      <c r="AI2">
+        <v>56.612000000000002</v>
+      </c>
+      <c r="AJ2">
+        <v>56.87166666666667</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>